<commit_message>
Mise à jour des prix et ajout d’images
</commit_message>
<xml_diff>
--- a/prix/bicone.xlsx
+++ b/prix/bicone.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\raccords-plomberie\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\raccords-plomberie\prix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4F0A4CA-8BF3-430C-92F2-AA9BBBD97C33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{889C7F3A-379B-4116-BC82-FF98161DBBEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="19416" windowHeight="11016" xr2:uid="{CE534A2A-185F-4964-A8EA-80A75C3E7C34}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CE534A2A-185F-4964-A8EA-80A75C3E7C34}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="181">
   <si>
     <t>43107100</t>
   </si>
@@ -498,6 +498,87 @@
   </si>
   <si>
     <t>Article</t>
+  </si>
+  <si>
+    <t>Denomination</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>12-10</t>
+  </si>
+  <si>
+    <t>15-10</t>
+  </si>
+  <si>
+    <t>15-12</t>
+  </si>
+  <si>
+    <t>1/2F-12</t>
+  </si>
+  <si>
+    <t>3/4F-15</t>
+  </si>
+  <si>
+    <t>3/8F-10</t>
+  </si>
+  <si>
+    <t>3/8F-12</t>
+  </si>
+  <si>
+    <t>1/2F-15</t>
+  </si>
+  <si>
+    <t>3/4F-22</t>
+  </si>
+  <si>
+    <t>3/4F-18</t>
+  </si>
+  <si>
+    <t>1/2F-10</t>
+  </si>
+  <si>
+    <t>1/2M-12</t>
+  </si>
+  <si>
+    <t>1/2M-15</t>
+  </si>
+  <si>
+    <t>3/4M-15</t>
+  </si>
+  <si>
+    <t>3/4M-18</t>
+  </si>
+  <si>
+    <t>3/4M-22</t>
+  </si>
+  <si>
+    <t>1/-15</t>
+  </si>
+  <si>
+    <t>1/-12</t>
   </si>
 </sst>
 </file>
@@ -909,1034 +990,1251 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E4F7123-4CF8-49A4-855C-11A40771464A}">
-  <dimension ref="A1:K72"/>
+  <dimension ref="A1:L72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="B79" sqref="B79"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="24.44140625" style="6" customWidth="1"/>
     <col min="2" max="2" width="51.77734375" style="8" customWidth="1"/>
-    <col min="3" max="3" width="11.77734375" style="9" customWidth="1"/>
-    <col min="4" max="4" width="22.77734375" style="8" customWidth="1"/>
-    <col min="6" max="6" width="23.77734375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="11.77734375" style="2" customWidth="1"/>
-    <col min="9" max="10" width="21.77734375" style="2" customWidth="1"/>
-    <col min="11" max="11" width="26.77734375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="7.77734375" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.77734375" style="9" customWidth="1"/>
+    <col min="5" max="5" width="22.77734375" style="8" customWidth="1"/>
+    <col min="7" max="7" width="23.77734375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.77734375" style="2" customWidth="1"/>
+    <col min="10" max="11" width="21.77734375" style="2" customWidth="1"/>
+    <col min="12" max="12" width="26.77734375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>144</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="H1" s="1"/>
+      <c r="G1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L1" s="1"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>142</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="9">
+      <c r="C2" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="D2" s="9">
         <v>4.07</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="E2" s="8" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>142</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="D3" s="9">
         <v>4.3899999999999997</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="E3" s="8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>142</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="D4" s="9">
         <v>4.0200000000000005</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="E4" s="8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>142</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="D5" s="9">
         <v>4.04</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="E5" s="8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>142</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="D6" s="9">
         <v>4.16</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="E6" s="8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>142</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="D7" s="9">
         <v>6.46</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="E7" s="8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>142</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="D8" s="9">
         <v>6.75</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="E8" s="8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>142</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="D9" s="9">
         <v>10.83</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="E9" s="8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>142</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="D10" s="9">
         <v>5.36</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="E10" s="8" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>142</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="D11" s="9">
         <v>4.0200000000000005</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="E11" s="8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>142</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D12" s="9">
         <v>5.19</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="E12" s="8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>143</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="D13" s="9">
         <v>2.57</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="E13" s="8" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>143</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="9">
+      <c r="C14" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="D14" s="9">
         <v>3.8200000000000003</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="E14" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>143</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="9">
+      <c r="C15" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="D15" s="9">
         <v>3.8200000000000003</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="E15" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>143</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="9">
+      <c r="C16" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="D16" s="9">
         <v>10.950000000000001</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="E16" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
         <v>143</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="9">
+      <c r="C17" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="D17" s="9">
         <v>4.5</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="E17" s="8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
         <v>143</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="9">
+      <c r="C18" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="D18" s="9">
         <v>5.21</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="E18" s="8" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
         <v>143</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C19" s="9">
+      <c r="C19" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="D19" s="9">
         <v>6.82</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="E19" s="8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
         <v>143</v>
       </c>
       <c r="B20" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="9">
+      <c r="C20" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="D20" s="9">
         <v>9.67</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="E20" s="8" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
         <v>145</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="9">
+      <c r="C21" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="D21" s="9">
         <v>5.93</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="E21" s="8" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
         <v>145</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C22" s="9">
+      <c r="C22" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="D22" s="9">
         <v>4.88</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="E22" s="8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
         <v>145</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C23" s="9">
+      <c r="C23" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="D23" s="9">
         <v>5.78</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="E23" s="8" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
         <v>145</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C24" s="9">
+      <c r="C24" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="D24" s="9">
         <v>6.3500000000000005</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="E24" s="8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
         <v>145</v>
       </c>
       <c r="B25" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C25" s="9">
+      <c r="C25" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="D25" s="9">
         <v>6.1000000000000005</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="E25" s="8" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
         <v>145</v>
       </c>
       <c r="B26" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="C26" s="9">
+      <c r="C26" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="D26" s="9">
         <v>10.33</v>
       </c>
-      <c r="D26" s="8" t="s">
+      <c r="E26" s="8" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
         <v>145</v>
       </c>
       <c r="B27" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C27" s="9">
+      <c r="C27" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="D27" s="9">
         <v>7.9</v>
       </c>
-      <c r="D27" s="8" t="s">
+      <c r="E27" s="8" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="s">
         <v>145</v>
       </c>
       <c r="B28" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C28" s="9">
+      <c r="C28" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="D28" s="9">
         <v>20.059999999999999</v>
       </c>
-      <c r="D28" s="8" t="s">
+      <c r="E28" s="8" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
         <v>146</v>
       </c>
       <c r="B29" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="C29" s="9">
+      <c r="C29" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="D29" s="9">
         <v>7.48</v>
       </c>
-      <c r="D29" s="8" t="s">
+      <c r="E29" s="8" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="6" t="s">
         <v>146</v>
       </c>
       <c r="B30" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="C30" s="9">
+      <c r="C30" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="D30" s="9">
         <v>5.48</v>
       </c>
-      <c r="D30" s="8" t="s">
+      <c r="E30" s="8" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
         <v>146</v>
       </c>
       <c r="B31" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="9">
+      <c r="C31" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="D31" s="9">
         <v>3.44</v>
       </c>
-      <c r="D31" s="8" t="s">
+      <c r="E31" s="8" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
         <v>146</v>
       </c>
       <c r="B32" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="C32" s="9">
+      <c r="C32" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="D32" s="9">
         <v>4.1399999999999997</v>
       </c>
-      <c r="D32" s="8" t="s">
+      <c r="E32" s="8" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="6" t="s">
         <v>146</v>
       </c>
       <c r="B33" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="C33" s="9">
+      <c r="C33" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="D33" s="9">
         <v>5.25</v>
       </c>
-      <c r="D33" s="8" t="s">
+      <c r="E33" s="8" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="6" t="s">
         <v>146</v>
       </c>
       <c r="B34" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="C34" s="9">
+      <c r="C34" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="D34" s="9">
         <v>6.07</v>
       </c>
-      <c r="D34" s="8" t="s">
+      <c r="E34" s="8" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="6" t="s">
         <v>146</v>
       </c>
       <c r="B35" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="C35" s="9">
+      <c r="C35" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="D35" s="9">
         <v>5.0600000000000005</v>
       </c>
-      <c r="D35" s="8" t="s">
+      <c r="E35" s="8" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="6" t="s">
         <v>146</v>
       </c>
       <c r="B36" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="C36" s="9">
+      <c r="C36" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="D36" s="9">
         <v>5.26</v>
       </c>
-      <c r="D36" s="8" t="s">
+      <c r="E36" s="8" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="6" t="s">
         <v>147</v>
       </c>
       <c r="B37" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="C37" s="9">
+      <c r="C37" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="D37" s="9">
         <v>3.8200000000000003</v>
       </c>
-      <c r="D37" s="8" t="s">
+      <c r="E37" s="8" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="6" t="s">
         <v>147</v>
       </c>
       <c r="B38" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="C38" s="9">
+      <c r="C38" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="D38" s="9">
         <v>4.46</v>
       </c>
-      <c r="D38" s="8" t="s">
+      <c r="E38" s="8" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="6" t="s">
         <v>147</v>
       </c>
       <c r="B39" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="C39" s="9">
+      <c r="C39" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="D39" s="9">
         <v>5.0600000000000005</v>
       </c>
-      <c r="D39" s="8" t="s">
+      <c r="E39" s="8" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="6" t="s">
         <v>147</v>
       </c>
       <c r="B40" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="C40" s="9">
+      <c r="C40" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="D40" s="9">
         <v>5.0600000000000005</v>
       </c>
-      <c r="D40" s="8" t="s">
+      <c r="E40" s="8" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="6" t="s">
         <v>147</v>
       </c>
       <c r="B41" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="C41" s="9">
+      <c r="C41" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="D41" s="9">
         <v>8.32</v>
       </c>
-      <c r="D41" s="8" t="s">
+      <c r="E41" s="8" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="6" t="s">
         <v>148</v>
       </c>
       <c r="B42" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="C42" s="9">
+      <c r="C42" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="D42" s="9">
         <v>3.8000000000000003</v>
       </c>
-      <c r="D42" s="8" t="s">
+      <c r="E42" s="8" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="6" t="s">
         <v>148</v>
       </c>
       <c r="B43" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="C43" s="9">
+      <c r="C43" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="D43" s="9">
         <v>3.2600000000000002</v>
       </c>
-      <c r="D43" s="8" t="s">
+      <c r="E43" s="8" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="6" t="s">
         <v>148</v>
       </c>
       <c r="B44" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="C44" s="9">
+      <c r="C44" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="D44" s="9">
         <v>3.54</v>
       </c>
-      <c r="D44" s="8" t="s">
+      <c r="E44" s="8" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="6" t="s">
         <v>148</v>
       </c>
       <c r="B45" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="C45" s="9">
+      <c r="C45" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="D45" s="9">
         <v>3.8000000000000003</v>
       </c>
-      <c r="D45" s="8" t="s">
+      <c r="E45" s="8" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="6" t="s">
         <v>148</v>
       </c>
       <c r="B46" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="C46" s="9">
+      <c r="C46" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="D46" s="9">
         <v>4.38</v>
       </c>
-      <c r="D46" s="8" t="s">
+      <c r="E46" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="6" t="s">
         <v>148</v>
       </c>
       <c r="B47" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="C47" s="9">
+      <c r="C47" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="D47" s="9">
         <v>3.39</v>
       </c>
-      <c r="D47" s="8" t="s">
+      <c r="E47" s="8" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="6" t="s">
         <v>148</v>
       </c>
       <c r="B48" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="C48" s="9">
+      <c r="C48" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="D48" s="9">
         <v>4.09</v>
       </c>
-      <c r="D48" s="8" t="s">
+      <c r="E48" s="8" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="6" t="s">
         <v>148</v>
       </c>
       <c r="B49" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="C49" s="9">
+      <c r="C49" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="D49" s="9">
         <v>2.86</v>
       </c>
-      <c r="D49" s="8" t="s">
+      <c r="E49" s="8" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="6" t="s">
         <v>148</v>
       </c>
       <c r="B50" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="C50" s="9">
+      <c r="C50" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="D50" s="9">
         <v>3.34</v>
       </c>
-      <c r="D50" s="8" t="s">
+      <c r="E50" s="8" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="6" t="s">
         <v>148</v>
       </c>
       <c r="B51" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="C51" s="9">
+      <c r="C51" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="D51" s="9">
         <v>3.09</v>
       </c>
-      <c r="D51" s="8" t="s">
+      <c r="E51" s="8" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="6" t="s">
         <v>148</v>
       </c>
       <c r="B52" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="C52" s="9">
+      <c r="C52" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="D52" s="9">
         <v>4.6500000000000004</v>
       </c>
-      <c r="D52" s="8" t="s">
+      <c r="E52" s="8" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="6" t="s">
         <v>148</v>
       </c>
       <c r="B53" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="C53" s="9">
+      <c r="C53" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="D53" s="9">
         <v>5.67</v>
       </c>
-      <c r="D53" s="8" t="s">
+      <c r="E53" s="8" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="6" t="s">
         <v>148</v>
       </c>
       <c r="B54" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="C54" s="9">
+      <c r="C54" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="D54" s="9">
         <v>4.5</v>
       </c>
-      <c r="D54" s="8" t="s">
+      <c r="E54" s="8" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="6" t="s">
         <v>148</v>
       </c>
       <c r="B55" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="C55" s="9">
+      <c r="C55" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="D55" s="9">
         <v>9.34</v>
       </c>
-      <c r="D55" s="8" t="s">
+      <c r="E55" s="8" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="6" t="s">
         <v>148</v>
       </c>
       <c r="B56" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="C56" s="9">
+      <c r="C56" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="D56" s="9">
         <v>9.9600000000000009</v>
       </c>
-      <c r="D56" s="8" t="s">
+      <c r="E56" s="8" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="6" t="s">
         <v>149</v>
       </c>
       <c r="B57" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="C57" s="9">
+      <c r="C57" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="D57" s="9">
         <v>2.57</v>
       </c>
-      <c r="D57" s="8" t="s">
+      <c r="E57" s="8" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="6" t="s">
         <v>149</v>
       </c>
       <c r="B58" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="C58" s="9">
+      <c r="C58" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="D58" s="9">
         <v>2.5100000000000002</v>
       </c>
-      <c r="D58" s="8" t="s">
+      <c r="E58" s="8" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="6" t="s">
         <v>149</v>
       </c>
       <c r="B59" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="C59" s="9">
+      <c r="C59" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="D59" s="9">
         <v>2.7600000000000002</v>
       </c>
-      <c r="D59" s="8" t="s">
+      <c r="E59" s="8" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="6" t="s">
         <v>149</v>
       </c>
       <c r="B60" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="C60" s="9">
+      <c r="C60" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="D60" s="9">
         <v>3.48</v>
       </c>
-      <c r="D60" s="8" t="s">
+      <c r="E60" s="8" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="6" t="s">
         <v>149</v>
       </c>
       <c r="B61" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="C61" s="9">
+      <c r="C61" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="D61" s="9">
         <v>3.35</v>
       </c>
-      <c r="D61" s="8" t="s">
+      <c r="E61" s="8" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="6" t="s">
         <v>149</v>
       </c>
       <c r="B62" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="C62" s="9">
+      <c r="C62" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="D62" s="9">
         <v>4.1399999999999997</v>
       </c>
-      <c r="D62" s="8" t="s">
+      <c r="E62" s="8" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="6" t="s">
         <v>149</v>
       </c>
       <c r="B63" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="C63" s="9">
+      <c r="C63" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="D63" s="9">
         <v>3.22</v>
       </c>
-      <c r="D63" s="8" t="s">
+      <c r="E63" s="8" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="6" t="s">
         <v>149</v>
       </c>
       <c r="B64" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="C64" s="9">
+      <c r="C64" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="D64" s="9">
         <v>3.34</v>
       </c>
-      <c r="D64" s="8" t="s">
+      <c r="E64" s="8" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="6" t="s">
         <v>149</v>
       </c>
       <c r="B65" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="C65" s="9">
+      <c r="C65" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="D65" s="9">
         <v>3.34</v>
       </c>
-      <c r="D65" s="8" t="s">
+      <c r="E65" s="8" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="6" t="s">
         <v>149</v>
       </c>
       <c r="B66" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="C66" s="9">
+      <c r="C66" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="D66" s="9">
         <v>3.19</v>
       </c>
-      <c r="D66" s="8" t="s">
+      <c r="E66" s="8" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" s="6" t="s">
         <v>149</v>
       </c>
       <c r="B67" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="C67" s="9">
+      <c r="C67" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="D67" s="9">
         <v>4.79</v>
       </c>
-      <c r="D67" s="8" t="s">
+      <c r="E67" s="8" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" s="6" t="s">
         <v>149</v>
       </c>
       <c r="B68" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="C68" s="9">
+      <c r="C68" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="D68" s="9">
         <v>5.67</v>
       </c>
-      <c r="D68" s="8" t="s">
+      <c r="E68" s="8" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="6" t="s">
         <v>149</v>
       </c>
       <c r="B69" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="C69" s="9">
+      <c r="C69" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="D69" s="9">
         <v>5.18</v>
       </c>
-      <c r="D69" s="8" t="s">
+      <c r="E69" s="8" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" s="6" t="s">
         <v>149</v>
       </c>
       <c r="B70" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="C70" s="9">
+      <c r="C70" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="D70" s="9">
         <v>10.57</v>
       </c>
-      <c r="D70" s="8" t="s">
+      <c r="E70" s="8" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" s="6" t="s">
         <v>150</v>
       </c>
       <c r="B71" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="C71" s="9">
+      <c r="C71" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="D71" s="9">
         <v>6.28</v>
       </c>
-      <c r="D71" s="8" t="s">
+      <c r="E71" s="8" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" s="6" t="s">
         <v>150</v>
       </c>
       <c r="B72" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="C72" s="9">
+      <c r="C72" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="D72" s="9">
         <v>4.9800000000000004</v>
       </c>
-      <c r="D72" s="8" t="s">
+      <c r="E72" s="8" t="s">
         <v>140</v>
       </c>
     </row>

</xml_diff>